<commit_message>
HALT translation template for the project
</commit_message>
<xml_diff>
--- a/HALT_dict_to_translate.xlsx
+++ b/HALT_dict_to_translate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanderki\Documents\vocaloidproject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Kilian\Documents\R-Projekte\vocaloidproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3D57B0-9E7E-4D41-9C37-E3C739E09CCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1488D57B-3EB3-4B11-9757-ADE61DA4E093}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="152">
   <si>
     <t>key</t>
   </si>
@@ -494,6 +494,18 @@
   </si>
   <si>
     <t>Unfortunately, your input was wrong. The playback volume is probably too low. You can increase the volume by the smallest possible value and then repeat the task.</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>relevant to vocaloid project</t>
+  </si>
+  <si>
+    <t>not currently</t>
   </si>
 </sst>
 </file>
@@ -880,53 +892,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="4" width="45.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="5" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>149</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
       </c>
       <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>149</v>
       </c>
       <c r="C3" t="s">
         <v>48</v>
@@ -934,592 +956,721 @@
       <c r="D3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
       <c r="B4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>149</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
       <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>149</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
       </c>
       <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>149</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
       <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
       <c r="B11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>31</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
       <c r="B12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>35</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>52</v>
       </c>
       <c r="B13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13" t="s">
         <v>53</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>54</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>149</v>
       </c>
       <c r="C14" t="s">
         <v>50</v>
       </c>
       <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
       <c r="B15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" t="s">
         <v>57</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>58</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>
       <c r="B16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" t="s">
         <v>61</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>62</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>136</v>
       </c>
       <c r="B18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C18" t="s">
         <v>137</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>138</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>140</v>
       </c>
       <c r="B19" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" t="s">
         <v>141</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>142</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>144</v>
       </c>
       <c r="B20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" t="s">
         <v>145</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>146</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>149</v>
       </c>
       <c r="C21" t="s">
         <v>71</v>
       </c>
       <c r="D21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>149</v>
       </c>
       <c r="C22" t="s">
         <v>65</v>
       </c>
       <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="C23" t="s">
         <v>68</v>
       </c>
       <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>73</v>
       </c>
       <c r="B24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" t="s">
         <v>74</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>75</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>89</v>
       </c>
       <c r="B25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" t="s">
         <v>90</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>91</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>151</v>
       </c>
       <c r="C26" t="s">
         <v>78</v>
       </c>
       <c r="D26" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
       <c r="C27" t="s">
         <v>81</v>
       </c>
       <c r="D27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="C28" t="s">
         <v>84</v>
       </c>
       <c r="D28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>86</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>151</v>
       </c>
       <c r="C29" t="s">
         <v>87</v>
       </c>
       <c r="D29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>105</v>
       </c>
       <c r="B30" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30" t="s">
         <v>106</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>107</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>93</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="C31" t="s">
         <v>94</v>
       </c>
       <c r="D31" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>96</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
       <c r="C32" t="s">
         <v>97</v>
       </c>
       <c r="D32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>100</v>
+        <v>151</v>
       </c>
       <c r="C33" t="s">
         <v>100</v>
       </c>
       <c r="D33" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>102</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
       <c r="C34" t="s">
         <v>103</v>
       </c>
       <c r="D34" t="s">
+        <v>103</v>
+      </c>
+      <c r="E34" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>109</v>
       </c>
       <c r="B35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C35" t="s">
         <v>110</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>111</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>113</v>
       </c>
       <c r="B36" t="s">
+        <v>151</v>
+      </c>
+      <c r="C36" t="s">
         <v>110</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>114</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>116</v>
       </c>
       <c r="B37" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" t="s">
         <v>110</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>117</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>119</v>
       </c>
       <c r="B38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C38" t="s">
         <v>110</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>117</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>120</v>
       </c>
       <c r="B39" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" t="s">
         <v>57</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>121</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>132</v>
       </c>
       <c r="B40" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" t="s">
         <v>133</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>134</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>123</v>
       </c>
       <c r="B41" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="C41" t="s">
         <v>124</v>
       </c>
       <c r="D41" t="s">
+        <v>124</v>
+      </c>
+      <c r="E41" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>126</v>
       </c>
       <c r="B42" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="C42" t="s">
         <v>127</v>
       </c>
       <c r="D42" t="s">
+        <v>127</v>
+      </c>
+      <c r="E42" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>129</v>
       </c>
       <c r="B43" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="C43" t="s">
         <v>130</v>
       </c>
       <c r="D43" t="s">
+        <v>130</v>
+      </c>
+      <c r="E43" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>149</v>
       </c>
       <c r="C44" t="s">
         <v>38</v>
       </c>
       <c r="D44" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>40</v>
       </c>
       <c r="B45" t="s">
+        <v>149</v>
+      </c>
+      <c r="C45" t="s">
         <v>41</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>42</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>